<commit_message>
CSV file converted with XLXS file for excel format to preserve All formatting for next use data'
</commit_message>
<xml_diff>
--- a/practice_sales_data.xlsx
+++ b/practice_sales_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\GitHub\Excel-Advance-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0899F91B-107A-475D-BD93-FB81737F06DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E20FB136-2F87-49DA-B6C6-E807DD5AD6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,16 +259,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">

</xml_diff>